<commit_message>
Update for info files
</commit_message>
<xml_diff>
--- a/info/South-Subassembly-Cameras.xlsx
+++ b/info/South-Subassembly-Cameras.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berriers\Documents\PARSEC Programming\nodejs-canon-control-client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berriers\Documents\PARSEC Programming\nodejs-canon-control-client\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84DB3154-4B4C-4C70-9351-0E9AE7959794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EF473E-8D9C-4C09-B778-3E998C51CDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-4575" windowWidth="13740" windowHeight="23640" xr2:uid="{B86F6753-CF77-493D-9452-DF2E8E254C20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B86F6753-CF77-493D-9452-DF2E8E254C20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4971E2-6F06-418A-B3E8-A5F21845BE12}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Switched to tabbed interface
</commit_message>
<xml_diff>
--- a/info/South-Subassembly-Cameras.xlsx
+++ b/info/South-Subassembly-Cameras.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berriers\Documents\PARSEC Programming\nodejs-canon-control-client\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EF473E-8D9C-4C09-B778-3E998C51CDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1C7A6E-E52C-49CF-90FA-3E2878286E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B86F6753-CF77-493D-9452-DF2E8E254C20}"/>
   </bookViews>
@@ -214,8 +214,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BD94F15-43F4-48BD-9231-4D9572C0AD2E}" name="Table1" displayName="Table1" ref="A1:C27" totalsRowShown="0">
   <autoFilter ref="A1:C27" xr:uid="{9BD94F15-43F4-48BD-9231-4D9572C0AD2E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C26">
-    <sortCondition ref="A1:A26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C27">
+    <sortCondition ref="C1:C27"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{54E80D7B-ACE9-4E87-8FA7-9D78D5C955DA}" name="Index"/>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4971E2-6F06-418A-B3E8-A5F21845BE12}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,13 +549,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
-        <v>62070106229</v>
+        <v>12070007710</v>
       </c>
       <c r="G2" t="s">
         <v>30</v>
@@ -563,70 +563,70 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>32070031166</v>
+        <v>12070010737</v>
       </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1">
-        <v>52070001320</v>
+        <v>12070029657</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
-        <v>22070055293</v>
+        <v>22070051119</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1">
-        <v>32070074172</v>
+        <v>22070055293</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
-        <v>12070029657</v>
+        <v>32070003759</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1">
-        <v>32070062372</v>
+        <v>32070010736</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -643,190 +643,190 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1">
-        <v>52070043886</v>
+        <v>32070031166</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1">
-        <v>42070018720</v>
+        <v>32070057845</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1">
-        <v>42070016637</v>
+        <v>32070062372</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1">
-        <v>22070051119</v>
+        <v>32070062451</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1">
-        <v>32070010736</v>
+        <v>32070074172</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1">
-        <v>32070003759</v>
+        <v>42070016637</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1">
-        <v>62070021384</v>
+        <v>42070018720</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1">
-        <v>12070007710</v>
+        <v>42070049368</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
       </c>
       <c r="C18" s="1">
-        <v>52070083924</v>
+        <v>52070001320</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1">
-        <v>42070049368</v>
+        <v>52070043886</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1">
-        <v>12070010737</v>
+        <v>52070044337</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1">
-        <v>62070106250</v>
+        <v>52070070569</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C22" s="1">
-        <v>62070018477</v>
+        <v>52070083924</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1">
-        <v>32070062451</v>
+        <v>62070018477</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1">
-        <v>52070070569</v>
+        <v>62070021384</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1">
-        <v>32070057845</v>
+        <v>62070106229</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1">
-        <v>52070044337</v>
+        <v>62070106250</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>